<commit_message>
Vergleichsgrafiken überarbeitet; Randomforest Plot erzeugt
</commit_message>
<xml_diff>
--- a/Ergebnisse/Excel/Mittelwerte/Items.xlsx
+++ b/Ergebnisse/Excel/Mittelwerte/Items.xlsx
@@ -491,7 +491,7 @@
     <t xml:space="preserve">Settings.Ex</t>
   </si>
   <si>
-    <t xml:space="preserve">Fallkomm.ext.Dialog.KJP </t>
+    <t xml:space="preserve">Fallkomm.ext.Dialog.KJP</t>
   </si>
   <si>
     <t xml:space="preserve">F555_13</t>
@@ -545,7 +545,7 @@
     <t xml:space="preserve">m) Krisenaufarbeitung: m) Bei Entlassungen aus der KJP (nach einer krisenhaften Aufnahme) muss ein Entlassgespräch zwischen KJP und mindestens einem Mitglied des Betreuungs-Teams geführt werden.</t>
   </si>
   <si>
-    <t xml:space="preserve">Fallkomm.ext.JA </t>
+    <t xml:space="preserve">Fallkomm.ext.JA</t>
   </si>
   <si>
     <t xml:space="preserve">F504_01</t>
@@ -2003,7 +2003,7 @@
     <t xml:space="preserve">Fortbildungen: Autorität durch Beziehung</t>
   </si>
   <si>
-    <t xml:space="preserve">MA.Supervis.FD/BL</t>
+    <t xml:space="preserve">MA.Supervis.FD_BL</t>
   </si>
   <si>
     <t xml:space="preserve">I910_03</t>

</xml_diff>